<commit_message>
added smarter product catalog added search added increment/decrement product quantity added some minor improvements
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
+++ b/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>Stories</t>
   </si>
@@ -317,6 +313,18 @@
   </si>
   <si>
     <t>Wer</t>
+  </si>
+  <si>
+    <t>Kai</t>
+  </si>
+  <si>
+    <t>Partymarti</t>
+  </si>
+  <si>
+    <t>Riedo</t>
+  </si>
+  <si>
+    <t>Alle</t>
   </si>
 </sst>
 </file>
@@ -660,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,6 +762,9 @@
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -765,6 +776,9 @@
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -776,6 +790,9 @@
       <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -787,6 +804,9 @@
       <c r="C12" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -809,6 +829,9 @@
       <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -820,6 +843,9 @@
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -831,8 +857,11 @@
       <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -842,8 +871,11 @@
       <c r="C17" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -853,8 +885,11 @@
       <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -864,8 +899,11 @@
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -875,8 +913,11 @@
       <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -886,8 +927,11 @@
       <c r="C21" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -897,8 +941,11 @@
       <c r="C22" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -908,8 +955,11 @@
       <c r="C23" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -919,8 +969,11 @@
       <c r="C24" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -930,8 +983,11 @@
       <c r="C25" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -941,8 +997,11 @@
       <c r="C26" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="D26" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>56</v>
       </c>
@@ -952,8 +1011,11 @@
       <c r="C27" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D27" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
@@ -963,8 +1025,11 @@
       <c r="C28" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -974,8 +1039,11 @@
       <c r="C29" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -985,8 +1053,11 @@
       <c r="C30" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -996,8 +1067,11 @@
       <c r="C31" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
@@ -1007,8 +1081,11 @@
       <c r="C32" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -1018,8 +1095,11 @@
       <c r="C33" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1029,8 +1109,11 @@
       <c r="C34" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -1041,7 +1124,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -1050,6 +1133,9 @@
       </c>
       <c r="C36" s="4" t="s">
         <v>52</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added DB connection changed catalog to use DB connection changed login to use DB connection
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
+++ b/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
   <si>
     <t>Stories</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>Alle</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -666,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,12 +685,12 @@
     <col min="3" max="3" width="69" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -697,8 +703,11 @@
       <c r="D2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -709,7 +718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -720,7 +729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
@@ -731,7 +740,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -742,17 +751,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -766,7 +775,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -780,7 +789,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -794,7 +803,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -808,7 +817,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -819,7 +828,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -833,7 +842,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -847,7 +856,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -861,7 +870,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -875,7 +884,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -889,7 +898,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -903,7 +912,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -917,7 +926,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -931,7 +940,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -945,7 +954,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -959,7 +968,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -973,7 +982,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -987,7 +996,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -1001,7 +1010,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>56</v>
       </c>
@@ -1015,7 +1024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
@@ -1029,7 +1038,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1043,7 +1052,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -1057,7 +1066,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -1070,8 +1079,11 @@
       <c r="D31" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
@@ -1084,8 +1096,11 @@
       <c r="D32" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -1098,8 +1113,11 @@
       <c r="D33" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1113,7 +1131,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -1124,7 +1142,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
fixed multilingual added standard template engine began with fixing soap service response interpretation
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
+++ b/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>Stories</t>
   </si>
@@ -312,9 +312,6 @@
     <t>Kai</t>
   </si>
   <si>
-    <t>Partymarti</t>
-  </si>
-  <si>
     <t>Riedo</t>
   </si>
   <si>
@@ -328,6 +325,12 @@
   </si>
   <si>
     <t>begonnen</t>
+  </si>
+  <si>
+    <t>obsolet</t>
+  </si>
+  <si>
+    <t>alle</t>
   </si>
 </sst>
 </file>
@@ -671,14 +674,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="69" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -701,7 +704,7 @@
         <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -714,6 +717,9 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -725,6 +731,9 @@
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="E4" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -747,6 +756,9 @@
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -761,6 +773,9 @@
       <c r="D7" t="s">
         <v>58</v>
       </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -775,6 +790,9 @@
       <c r="D8" t="s">
         <v>58</v>
       </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -787,7 +805,10 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -804,7 +825,7 @@
         <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="150" x14ac:dyDescent="0.25">
@@ -817,6 +838,9 @@
       <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -832,7 +856,7 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="210" x14ac:dyDescent="0.25">
@@ -846,7 +870,10 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -860,7 +887,10 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -874,7 +904,10 @@
         <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -888,7 +921,7 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -902,7 +935,7 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -916,7 +949,7 @@
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -930,7 +963,7 @@
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -944,7 +977,7 @@
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -958,7 +991,7 @@
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -972,7 +1005,7 @@
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -986,7 +1019,7 @@
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -1000,7 +1033,7 @@
         <v>31</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1014,7 +1047,7 @@
         <v>53</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1028,7 +1061,7 @@
         <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1042,7 +1075,7 @@
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1056,7 +1089,7 @@
         <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1073,7 +1106,7 @@
         <v>58</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1090,7 +1123,7 @@
         <v>58</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1107,7 +1140,7 @@
         <v>58</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1124,7 +1157,7 @@
         <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1137,6 +1170,12 @@
       <c r="C33" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="34" spans="1:5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -1149,7 +1188,7 @@
         <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed tasklist extended webservice added images
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
+++ b/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$34</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
   <si>
     <t>Stories</t>
   </si>
@@ -672,10 +675,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +750,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -759,8 +763,11 @@
       <c r="D6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -777,7 +784,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -794,7 +801,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -811,7 +818,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -828,7 +835,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:5" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -842,7 +849,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -859,7 +866,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:5" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -876,7 +883,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -893,7 +900,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1050,7 +1057,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1063,8 +1070,11 @@
       <c r="D26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1076,6 +1086,9 @@
       </c>
       <c r="D27" t="s">
         <v>59</v>
+      </c>
+      <c r="E27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1092,7 +1105,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
@@ -1109,7 +1122,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -1126,7 +1139,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -1160,7 +1173,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
@@ -1174,7 +1187,7 @@
         <v>58</v>
       </c>
       <c r="E33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1198,6 +1211,14 @@
       <c r="C36" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:E34">
+    <filterColumn colId="4">
+      <filters blank="1">
+        <filter val="begonnen"/>
+        <filter val="obsolet"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added template engine for products tweaked some design stuff like footer
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
+++ b/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
   <si>
     <t>Stories</t>
   </si>
@@ -679,7 +679,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +751,9 @@
       </c>
       <c r="D5" s="6" t="s">
         <v>58</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix for confimation page
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
+++ b/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="6780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -678,8 +678,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
readded tasks.xlsx changed präsi
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
+++ b/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\shop\ch.bfh.bti7054.w2014.p.pc-hammer\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$34</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -676,7 +680,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
@@ -770,7 +774,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -787,7 +791,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -804,7 +808,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -821,7 +825,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -838,7 +842,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:5" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -852,7 +856,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -869,7 +873,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:5" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -886,7 +890,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -903,7 +907,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -920,7 +924,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -934,7 +938,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -948,7 +952,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -962,7 +966,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -976,7 +980,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>23</v>
       </c>
@@ -990,7 +994,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1018,7 +1022,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1060,7 +1064,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:5" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1077,7 +1081,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:5" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1094,7 +1098,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
@@ -1108,7 +1112,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
@@ -1125,7 +1129,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:5" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -1142,7 +1146,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:5" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -1159,7 +1163,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
@@ -1176,7 +1180,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
@@ -1193,7 +1197,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
@@ -1206,12 +1210,6 @@
       <c r="D34" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:E34">

</xml_diff>

<commit_message>
added contact form, update excel and ppt
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
+++ b/ch.bfh.bti7054.w2014.p.pc-hammer/doc/Tasks.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webprogramming\ch.bfh.bti7054.w2014.p.pc-hammer\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$37</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="73">
   <si>
     <t>HTML Struktur</t>
   </si>
@@ -273,15 +278,6 @@
     <t>Tasks</t>
   </si>
   <si>
-    <t>options and email</t>
-  </si>
-  <si>
-    <t>more classes for cart items</t>
-  </si>
-  <si>
-    <t>at finish line</t>
-  </si>
-  <si>
     <t>not finished</t>
   </si>
   <si>
@@ -311,9 +307,6 @@
   </si>
   <si>
     <t>Create installation guide</t>
-  </si>
-  <si>
-    <t>create user</t>
   </si>
   <si>
     <t>Create powerpoint</t>
@@ -356,6 +349,9 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Marti</t>
   </si>
 </sst>
 </file>
@@ -472,9 +468,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Berechnung" xfId="1" builtinId="22"/>
-    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -492,7 +488,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-CH"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -536,6 +532,13 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -543,6 +546,11 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -565,10 +573,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -903,7 +911,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -913,17 +921,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="73.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.42578125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="22.28515625" customWidth="1"/>
     <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -950,14 +957,14 @@
       </c>
       <c r="F2">
         <f>SUM(F3:F37)</f>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G2">
         <f>SUM(G3:G37)</f>
         <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K2">
         <f>G2</f>
@@ -975,9 +982,11 @@
         <v>2.1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>54</v>
       </c>
@@ -990,15 +999,15 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K3">
         <f>F2</f>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L3" s="13">
         <f>F2/G2</f>
-        <v>0.74285714285714288</v>
+        <v>0.97142857142857142</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1011,7 +1020,9 @@
       <c r="C4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="E4" s="9" t="s">
         <v>54</v>
       </c>
@@ -1024,15 +1035,15 @@
         <v>1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K4" s="3">
         <f>K2-K3</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="L4" s="14">
         <f>K4/K2</f>
-        <v>0.25714285714285712</v>
+        <v>2.8571428571428571E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1118,7 +1129,7 @@
         <v>4.2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>50</v>
@@ -1195,7 +1206,9 @@
       <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="E11" s="4" t="s">
         <v>54</v>
       </c>
@@ -1216,7 +1229,7 @@
         <v>5.2</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>50</v>
@@ -1241,7 +1254,7 @@
         <v>5.3</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>50</v>
@@ -1341,7 +1354,7 @@
         <v>6.2</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>51</v>
@@ -1397,11 +1410,11 @@
         <v>51</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
@@ -1447,11 +1460,11 @@
         <v>51</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
@@ -1472,11 +1485,11 @@
         <v>52</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
@@ -1508,7 +1521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
@@ -1516,7 +1529,7 @@
         <v>7.2</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>51</v>
@@ -1621,10 +1634,12 @@
       <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
@@ -1720,7 +1735,7 @@
         <v>50</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
@@ -1739,7 +1754,7 @@
         <v>11.1</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>50</v>
@@ -1767,12 +1782,14 @@
         <v>42</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
@@ -1781,19 +1798,23 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B35" s="9">
         <v>13.1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
@@ -1802,21 +1823,23 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B36" s="9">
         <v>13.2</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="E36" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
@@ -1825,19 +1848,23 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B37" s="9">
         <v>13.3</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>

</xml_diff>